<commit_message>
study2 data updated (Kathy)
</commit_message>
<xml_diff>
--- a/DC MOTOR/Applicaton/Boxer Game/Results/Study2_Questionnaire_Results.xlsx
+++ b/DC MOTOR/Applicaton/Boxer Game/Results/Study2_Questionnaire_Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>代稱</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -103,6 +103,46 @@
   </si>
   <si>
     <t>姓名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>唐千琳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kathy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>女</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一個月前</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>輕重</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>輕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>無</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>平均</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -110,7 +150,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -126,8 +166,17 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,6 +201,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -167,7 +222,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -178,6 +233,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -460,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O3"/>
+  <dimension ref="A2:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -478,101 +536,259 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <v>24</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" t="s">
         <v>17</v>
       </c>
-      <c r="H3">
+      <c r="H4">
         <v>2</v>
       </c>
-      <c r="I3">
+      <c r="I4">
         <v>2</v>
       </c>
-      <c r="J3">
+      <c r="J4">
         <v>4.5</v>
       </c>
-      <c r="K3">
+      <c r="K4">
         <v>4</v>
       </c>
-      <c r="L3">
+      <c r="L4">
         <v>5</v>
       </c>
-      <c r="M3">
+      <c r="M4">
         <v>5</v>
       </c>
-      <c r="N3">
+      <c r="N4">
         <v>4.5</v>
       </c>
-      <c r="O3">
+      <c r="O4">
         <v>4.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="M5">
+        <v>4</v>
+      </c>
+      <c r="N5">
+        <v>5</v>
+      </c>
+      <c r="O5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4">
+        <f>AVERAGE(E4:E15)</f>
+        <v>24.5</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="4">
+        <f>AVERAGE(H4:H15)</f>
+        <v>2.5</v>
+      </c>
+      <c r="I16" s="4">
+        <f t="shared" ref="I16:O16" si="0">AVERAGE(I4:I15)</f>
+        <v>2</v>
+      </c>
+      <c r="J16" s="4">
+        <f t="shared" si="0"/>
+        <v>4.25</v>
+      </c>
+      <c r="K16" s="4">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="L16" s="4">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="M16" s="4">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="N16" s="4">
+        <f t="shared" si="0"/>
+        <v>4.75</v>
+      </c>
+      <c r="O16" s="4">
+        <f t="shared" si="0"/>
+        <v>3.75</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Boxer disppear! -> fixed ; study2 data(wakeup & Rong) updated
</commit_message>
<xml_diff>
--- a/DC MOTOR/Applicaton/Boxer Game/Results/Study2_Questionnaire_Results.xlsx
+++ b/DC MOTOR/Applicaton/Boxer Game/Results/Study2_Questionnaire_Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_LabProject\NILab - FacePush\FacePush\DC MOTOR\Applicaton\Boxer Game\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_LabProject\NILab - FacePush\New folder\FacePush\DC MOTOR\Applicaton\Boxer Game\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="87">
   <si>
     <t>代稱</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -267,6 +267,133 @@
   </si>
   <si>
     <t>昨天</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蔡霈萱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>女</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WakeUp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>四個月前</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>真實度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>享受度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A&lt;B&lt;D=C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>受測後排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A&lt;B&lt;C&lt;D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A&lt;D&lt;B&lt;C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A&lt;B&lt;C&lt;D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A&lt;B=C&lt;D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蔡德蓉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>兩個月前</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A&lt;&lt;B=D&lt;C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A&lt;&lt;B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>≒</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D&lt;C</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A&lt;B&lt;D&lt;C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C=D=B=A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C=D&lt;B=A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A&lt;B=C=D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A&lt;B=C&lt;=D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A&lt;B=C=D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A&lt;D&lt;B&lt;C</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -274,7 +401,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -299,8 +426,31 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,6 +481,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -346,7 +502,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -360,6 +516,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -642,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P16"/>
+  <dimension ref="A2:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -656,11 +821,11 @@
     <col min="5" max="5" width="5" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
     <col min="7" max="7" width="15.875" customWidth="1"/>
-    <col min="8" max="15" width="11.625" customWidth="1"/>
-    <col min="16" max="16" width="13.75" customWidth="1"/>
+    <col min="8" max="17" width="11.625" customWidth="1"/>
+    <col min="18" max="18" width="13.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H2" t="s">
         <v>28</v>
       </c>
@@ -673,8 +838,11 @@
       <c r="N2" t="s">
         <v>26</v>
       </c>
+      <c r="P2" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -720,11 +888,17 @@
       <c r="O3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="P3" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -770,8 +944,14 @@
       <c r="O4">
         <v>4.5</v>
       </c>
+      <c r="P4" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -817,8 +997,14 @@
       <c r="O5">
         <v>3</v>
       </c>
+      <c r="P5" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -864,8 +1050,14 @@
       <c r="O6">
         <v>6</v>
       </c>
+      <c r="P6" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>83</v>
+      </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -908,8 +1100,14 @@
       <c r="O7">
         <v>3</v>
       </c>
+      <c r="P7" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>86</v>
+      </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -956,10 +1154,16 @@
         <v>5</v>
       </c>
       <c r="P8" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>85</v>
+      </c>
+      <c r="R8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1005,8 +1209,14 @@
       <c r="O9">
         <v>4.5</v>
       </c>
+      <c r="P9" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1052,8 +1262,14 @@
       <c r="O10">
         <v>6.5</v>
       </c>
+      <c r="P10" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q10" s="7" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1099,72 +1315,182 @@
       <c r="O11">
         <v>3</v>
       </c>
+      <c r="P11" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
+      <c r="B12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" t="s">
+        <v>77</v>
+      </c>
+      <c r="H12">
+        <v>5.2</v>
+      </c>
+      <c r="I12">
+        <v>6</v>
+      </c>
+      <c r="J12">
+        <v>6</v>
+      </c>
+      <c r="K12">
+        <v>6.3</v>
+      </c>
+      <c r="L12">
+        <v>6.5</v>
+      </c>
+      <c r="M12">
+        <v>6.7</v>
+      </c>
+      <c r="N12">
+        <v>6.1</v>
+      </c>
+      <c r="O12">
+        <v>6.4</v>
+      </c>
+      <c r="P12" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
+      <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13">
+        <v>24</v>
+      </c>
+      <c r="F13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="J13">
+        <v>3</v>
+      </c>
+      <c r="K13">
+        <v>5</v>
+      </c>
+      <c r="L13">
+        <v>3</v>
+      </c>
+      <c r="M13">
+        <v>5</v>
+      </c>
+      <c r="N13">
+        <v>5</v>
+      </c>
+      <c r="O13">
+        <v>5</v>
+      </c>
+      <c r="P13" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4">
-        <f>AVERAGE(E4:E15)</f>
-        <v>24</v>
-      </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4" t="s">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4">
+        <f>AVERAGE(E4:E16)</f>
+        <v>23.7</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H16" s="4">
-        <f>AVERAGE(H4:H15)</f>
-        <v>3.375</v>
-      </c>
-      <c r="I16" s="4">
-        <f t="shared" ref="I16:O16" si="0">AVERAGE(I4:I15)</f>
-        <v>3.125</v>
-      </c>
-      <c r="J16" s="4">
+      <c r="H17" s="4">
+        <f>AVERAGE(H4:H16)</f>
+        <v>3.4200000000000004</v>
+      </c>
+      <c r="I17" s="4">
+        <f t="shared" ref="I17:O17" si="0">AVERAGE(I4:I16)</f>
+        <v>3.5</v>
+      </c>
+      <c r="J17" s="4">
         <f t="shared" si="0"/>
-        <v>4.75</v>
-      </c>
-      <c r="K16" s="4">
+        <v>4.7</v>
+      </c>
+      <c r="K17" s="4">
         <f t="shared" si="0"/>
-        <v>4.625</v>
-      </c>
-      <c r="L16" s="4">
+        <v>4.83</v>
+      </c>
+      <c r="L17" s="4">
         <f t="shared" si="0"/>
-        <v>4.875</v>
-      </c>
-      <c r="M16" s="4">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="M17" s="4">
         <f t="shared" si="0"/>
-        <v>4.875</v>
-      </c>
-      <c r="N16" s="4">
+        <v>5.07</v>
+      </c>
+      <c r="N17" s="4">
         <f t="shared" si="0"/>
-        <v>4.6875</v>
-      </c>
-      <c r="O16" s="4">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="O17" s="4">
         <f t="shared" si="0"/>
-        <v>4.4375</v>
-      </c>
+        <v>4.6899999999999995</v>
+      </c>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
update study2 data (users*12 already)
</commit_message>
<xml_diff>
--- a/DC MOTOR/Applicaton/Boxer Game/Results/Study2_Questionnaire_Results.xlsx
+++ b/DC MOTOR/Applicaton/Boxer Game/Results/Study2_Questionnaire_Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_LabProject\NILab - FacePush\New folder\FacePush\DC MOTOR\Applicaton\Boxer Game\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_LabProject\NILab - FacePush\FacePush\DC MOTOR\Applicaton\Boxer Game\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="101">
   <si>
     <t>代稱</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -394,6 +394,62 @@
   </si>
   <si>
     <t>A&lt;D&lt;B&lt;C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>潘儀芳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mona</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>女</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>無</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A&lt;D&lt;C&lt;B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A&lt;B&lt;D&lt;C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>潘奕呈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Peter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>男</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一年前</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A&lt;C&lt;B&lt;D</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -810,7 +866,7 @@
   <dimension ref="A2:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1076,6 +1132,9 @@
       <c r="F7" t="s">
         <v>37</v>
       </c>
+      <c r="G7" t="s">
+        <v>93</v>
+      </c>
       <c r="H7">
         <v>2.5</v>
       </c>
@@ -1432,10 +1491,106 @@
       <c r="A14">
         <v>11</v>
       </c>
+      <c r="B14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E14">
+        <v>24</v>
+      </c>
+      <c r="F14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <v>6</v>
+      </c>
+      <c r="K14">
+        <v>5</v>
+      </c>
+      <c r="L14">
+        <v>6</v>
+      </c>
+      <c r="M14">
+        <v>6</v>
+      </c>
+      <c r="N14">
+        <v>6</v>
+      </c>
+      <c r="O14">
+        <v>6</v>
+      </c>
+      <c r="P14" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15">
+        <v>24</v>
+      </c>
+      <c r="F15" t="s">
+        <v>98</v>
+      </c>
+      <c r="G15" t="s">
+        <v>99</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15">
+        <v>5</v>
+      </c>
+      <c r="J15">
+        <v>6.2</v>
+      </c>
+      <c r="K15">
+        <v>6.5</v>
+      </c>
+      <c r="L15">
+        <v>6</v>
+      </c>
+      <c r="M15">
+        <v>6</v>
+      </c>
+      <c r="N15">
+        <v>6.5</v>
+      </c>
+      <c r="O15">
+        <v>7</v>
+      </c>
+      <c r="P15" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -1450,7 +1605,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4">
         <f>AVERAGE(E4:E16)</f>
-        <v>23.7</v>
+        <v>23.75</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4" t="s">
@@ -1458,35 +1613,35 @@
       </c>
       <c r="H17" s="4">
         <f>AVERAGE(H4:H16)</f>
-        <v>3.4200000000000004</v>
+        <v>3.2666666666666671</v>
       </c>
       <c r="I17" s="4">
         <f t="shared" ref="I17:O17" si="0">AVERAGE(I4:I16)</f>
-        <v>3.5</v>
+        <v>3.5833333333333335</v>
       </c>
       <c r="J17" s="4">
         <f t="shared" si="0"/>
-        <v>4.7</v>
+        <v>4.9333333333333336</v>
       </c>
       <c r="K17" s="4">
         <f t="shared" si="0"/>
-        <v>4.83</v>
+        <v>4.9833333333333334</v>
       </c>
       <c r="L17" s="4">
         <f t="shared" si="0"/>
-        <v>4.8499999999999996</v>
+        <v>5.041666666666667</v>
       </c>
       <c r="M17" s="4">
         <f t="shared" si="0"/>
-        <v>5.07</v>
+        <v>5.2250000000000005</v>
       </c>
       <c r="N17" s="4">
         <f t="shared" si="0"/>
-        <v>4.8600000000000003</v>
+        <v>5.0916666666666668</v>
       </c>
       <c r="O17" s="4">
         <f t="shared" si="0"/>
-        <v>4.6899999999999995</v>
+        <v>4.9916666666666663</v>
       </c>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>

</xml_diff>